<commit_message>
2e version du labyrinth
</commit_message>
<xml_diff>
--- a/Recap_exos_stage2.xlsx
+++ b/Recap_exos_stage2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UserData\Ludovic\Serieux\Scolaire\8.EPFL\Master\Semestre 4\Projet de semestre\First step\Stage 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UserData\Ludovic\Serieux\Scolaire\8.EPFL\Master\Semestre 4\Projet de semestre\First step\Stage 2\Debuggin-Tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC4B7D6-19C2-4192-B78A-9CB0E5453F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC62781-B26F-47F9-8E32-012F82012850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AC49E7E1-8857-4F13-9155-40FA21DFD908}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="125">
   <si>
     <t>Taches de debuggage</t>
   </si>
@@ -219,9 +219,6 @@
     <t>En VPL ou en scratch, mauvais seuil</t>
   </si>
   <si>
-    <t>Possible en VPL (preuve) et en scratch, utiliser les lumières pour les modes</t>
-  </si>
-  <si>
     <t>Pas possible en VPL ou en scratch -&gt; propre à python</t>
   </si>
   <si>
@@ -397,6 +394,12 @@
   </si>
   <si>
     <t>2 versions: avec des variables, et harcodé. Une novice m'a dit qu'elle preferait avoir les valeurs bruts (magic numbers / hardcodé)</t>
+  </si>
+  <si>
+    <t>2 versions: un grand labyrinth, plus complexe et plus interressant, et un plus petit, plus rapide, plus facile à debugger</t>
+  </si>
+  <si>
+    <t>Possible en VPL (preuve) et en scratch, utiliser les lumières pour les etats</t>
   </si>
 </sst>
 </file>
@@ -525,16 +528,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -545,6 +539,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -625,16 +628,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>71717</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>39059</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>279788</xdr:rowOff>
+      <xdr:rowOff>160045</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1205753</xdr:colOff>
+      <xdr:colOff>1817914</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>512221</xdr:rowOff>
+      <xdr:rowOff>583349</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -663,8 +666,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="71717" y="1005929"/>
-          <a:ext cx="1429871" cy="779280"/>
+          <a:off x="332973" y="1085331"/>
+          <a:ext cx="1778855" cy="967589"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -675,16 +678,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>195944</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>92136</xdr:rowOff>
+      <xdr:rowOff>48592</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1253079</xdr:colOff>
+      <xdr:colOff>1883230</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>845521</xdr:rowOff>
+      <xdr:rowOff>903864</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -713,8 +716,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="2100230"/>
-          <a:ext cx="1548914" cy="1120938"/>
+          <a:off x="489858" y="2247506"/>
+          <a:ext cx="1687286" cy="1225387"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -725,16 +728,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>156180</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>47323</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>557157</xdr:rowOff>
+      <xdr:rowOff>513614</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1179606</xdr:colOff>
+      <xdr:colOff>2093561</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>268045</xdr:rowOff>
+      <xdr:rowOff>468086</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -763,8 +766,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="156180" y="4031877"/>
-          <a:ext cx="1320606" cy="442408"/>
+          <a:off x="341237" y="3997043"/>
+          <a:ext cx="2046238" cy="683814"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -775,16 +778,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>179295</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>239485</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>31060</xdr:rowOff>
+      <xdr:rowOff>78491</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1981200</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>337510</xdr:rowOff>
+      <xdr:rowOff>468086</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -814,8 +817,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="179295" y="4603060"/>
-          <a:ext cx="1398494" cy="1041556"/>
+          <a:off x="533399" y="5205662"/>
+          <a:ext cx="1741715" cy="1118938"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -837,15 +840,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>88084</xdr:rowOff>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>860970</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1246095</xdr:colOff>
+      <xdr:colOff>2171403</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>191600</xdr:rowOff>
+      <xdr:rowOff>465909</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -868,8 +871,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="6130296"/>
-          <a:ext cx="1541930" cy="838623"/>
+          <a:off x="152400" y="7261770"/>
+          <a:ext cx="2312917" cy="1250859"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>27709</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>673621</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>724021</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>39830</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97BF4A44-28B1-713C-18FE-2A19331237EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="24910473" y="2128348"/>
+          <a:ext cx="2275730" cy="1375118"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1180,147 +1227,148 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB55087F-BEDA-4674-8F2A-2B3E9A08A28F}">
   <dimension ref="A2:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7:O8"/>
+    <sheetView tabSelected="1" topLeftCell="F6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.5546875" style="1"/>
     <col min="4" max="4" width="16.21875" style="1" customWidth="1"/>
     <col min="5" max="6" width="11.5546875" style="1"/>
-    <col min="7" max="7" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" style="1" customWidth="1"/>
     <col min="8" max="8" width="11.5546875" style="1"/>
     <col min="9" max="9" width="25.6640625" style="1" customWidth="1"/>
     <col min="10" max="13" width="11.5546875" style="1"/>
     <col min="14" max="14" width="22.44140625" style="1" customWidth="1"/>
     <col min="15" max="16" width="15.33203125" style="1" customWidth="1"/>
     <col min="17" max="17" width="22.33203125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="31.33203125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="32.77734375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="36.44140625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="39.88671875" style="1" customWidth="1"/>
     <col min="20" max="20" width="24.6640625" style="1" customWidth="1"/>
     <col min="21" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
       <c r="P2" s="9"/>
       <c r="Q2" s="9"/>
       <c r="R2" s="9"/>
       <c r="S2" s="9"/>
     </row>
     <row r="3" spans="1:20" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="11" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="H3" s="11" t="s">
+      <c r="G3" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="11" t="s">
+      <c r="N3" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="O3" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="P3" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q3" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="R3" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11" t="s">
+      <c r="P3" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q3" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="R3" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
       <c r="R4" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="S4" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="S4" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="T4" s="11"/>
+      <c r="T4" s="17"/>
     </row>
     <row r="5" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C5" s="11" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="12">
+      <c r="E5" s="11">
         <v>2</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>33</v>
       </c>
       <c r="G5" s="10" t="s">
@@ -1344,30 +1392,31 @@
       <c r="M5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N5" s="12" t="s">
+      <c r="N5" s="11" t="s">
         <v>52</v>
       </c>
       <c r="O5" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="P5" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q5" s="12" t="s">
-        <v>93</v>
+      <c r="P5" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q5" s="11" t="s">
+        <v>92</v>
       </c>
       <c r="R5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C6" s="11"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
       <c r="G6" s="10" t="s">
         <v>10</v>
       </c>
@@ -1389,37 +1438,38 @@
       <c r="M6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N6" s="12"/>
+      <c r="N6" s="11"/>
       <c r="O6" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
       <c r="R6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="S6" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C7" s="11" t="s">
+      <c r="B7" s="11"/>
+      <c r="C7" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="11">
         <v>2</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>19</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>20</v>
@@ -1427,39 +1477,43 @@
       <c r="J7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="L7" s="12" t="s">
+      <c r="K7" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="L7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="12" t="s">
+      <c r="M7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="N7" s="12" t="s">
+      <c r="N7" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="O7" s="15" t="s">
+      <c r="O7" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="P7" s="12" t="s">
-        <v>83</v>
+      <c r="P7" s="11" t="s">
+        <v>82</v>
       </c>
       <c r="Q7" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="S7" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="R7" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>96</v>
+      <c r="T7" s="11" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="72" x14ac:dyDescent="0.3">
-      <c r="C8" s="11"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
       <c r="G8" s="10" t="s">
         <v>21</v>
       </c>
@@ -1467,38 +1521,40 @@
         <v>11</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="12"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="11"/>
       <c r="Q8" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="R8" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="S8" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="S8" s="1" t="s">
-        <v>99</v>
-      </c>
+      <c r="T8" s="11"/>
     </row>
     <row r="9" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="11"/>
+      <c r="C9" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="11">
         <v>2</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G9" s="10" t="s">
@@ -1513,39 +1569,40 @@
       <c r="J9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="L9" s="12" t="s">
+      <c r="K9" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="L9" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="M9" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="N9" s="12" t="s">
+      <c r="M9" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="N9" s="11" t="s">
         <v>54</v>
       </c>
       <c r="O9" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="P9" s="12" t="s">
-        <v>84</v>
+      <c r="P9" s="11" t="s">
+        <v>83</v>
       </c>
       <c r="Q9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="R9" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="S9" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="72" x14ac:dyDescent="0.3">
-      <c r="C10" s="11"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
       <c r="G10" s="10" t="s">
         <v>24</v>
       </c>
@@ -1558,35 +1615,36 @@
       <c r="J10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
       <c r="O10" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="P10" s="12"/>
+      <c r="P10" s="11"/>
       <c r="Q10" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="R10" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="S10" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="S10" s="1" t="s">
-        <v>105</v>
-      </c>
     </row>
-    <row r="11" spans="1:20" ht="72" x14ac:dyDescent="0.3">
-      <c r="C11" s="11" t="s">
+    <row r="11" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="11"/>
+      <c r="C11" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="11">
         <v>2</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G11" s="10" t="s">
@@ -1601,39 +1659,40 @@
       <c r="J11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K11" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="L11" s="13" t="s">
+      <c r="K11" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="L11" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="M11" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="N11" s="12" t="s">
+      <c r="M11" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="N11" s="11" t="s">
         <v>55</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="P11" s="12" t="s">
-        <v>84</v>
+        <v>64</v>
+      </c>
+      <c r="P11" s="11" t="s">
+        <v>83</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="R11" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="S11" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="S11" s="1" t="s">
-        <v>107</v>
-      </c>
     </row>
-    <row r="12" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C12" s="11"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
+    <row r="12" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B12" s="11"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
       <c r="G12" s="10" t="s">
         <v>37</v>
       </c>
@@ -1646,87 +1705,87 @@
       <c r="J12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K12" s="12"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
       <c r="O12" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="P12" s="12"/>
+        <v>65</v>
+      </c>
+      <c r="P12" s="11"/>
       <c r="Q12" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="R12" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="R12" s="1" t="s">
+      <c r="S12" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="S12" s="1" t="s">
-        <v>111</v>
-      </c>
     </row>
-    <row r="13" spans="1:20" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B13" s="12"/>
-      <c r="C13" s="17" t="s">
+    <row r="13" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+      <c r="B13" s="11"/>
+      <c r="C13" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="E13" s="12">
+      <c r="D13" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="11">
         <v>3</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K13" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="L13" s="15" t="s">
+      <c r="K13" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="L13" s="12" t="s">
         <v>13</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N13" s="12" t="s">
+      <c r="N13" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="O13" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="P13" s="12" t="s">
-        <v>117</v>
+      <c r="O13" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="P13" s="11" t="s">
+        <v>116</v>
       </c>
       <c r="Q13" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R13" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="R13" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="S13" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="T13" s="12" t="s">
-        <v>123</v>
+        <v>118</v>
+      </c>
+      <c r="T13" s="11" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B14" s="12"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
       <c r="G14" s="10" t="s">
         <v>10</v>
       </c>
@@ -1734,36 +1793,36 @@
         <v>11</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K14" s="16"/>
-      <c r="L14" s="15"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="12"/>
       <c r="M14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N14" s="12"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="12"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="11"/>
       <c r="Q14" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R14" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="S14" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="S14" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="T14" s="12"/>
+      <c r="T14" s="11"/>
     </row>
     <row r="15" spans="1:20" ht="72" x14ac:dyDescent="0.3">
-      <c r="B15" s="12"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
       <c r="G15" s="10" t="s">
         <v>48</v>
       </c>
@@ -1776,34 +1835,75 @@
       <c r="J15" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K15" s="16"/>
-      <c r="L15" s="15"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="12"/>
       <c r="M15" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="N15" s="12"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="12"/>
+        <v>81</v>
+      </c>
+      <c r="N15" s="11"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="11"/>
       <c r="Q15" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="R15" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="R15" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="S15" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="T15" s="12"/>
+        <v>121</v>
+      </c>
+      <c r="T15" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="66">
-    <mergeCell ref="T13:T15"/>
-    <mergeCell ref="L13:L15"/>
-    <mergeCell ref="K13:K15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="D13:D15"/>
+  <mergeCells count="71">
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="P13:P15"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="B2:O2"/>
@@ -1820,49 +1920,13 @@
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="D5:D6"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="P13:P15"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="Q5:Q6"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="T13:T15"/>
+    <mergeCell ref="L13:L15"/>
+    <mergeCell ref="K13:K15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="D13:D15"/>
   </mergeCells>
   <conditionalFormatting sqref="J5:J12">
     <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="Moyen">

</xml_diff>